<commit_message>
First version of new models
</commit_message>
<xml_diff>
--- a/app/data/static/params/mozzarella.xlsx
+++ b/app/data/static/params/mozzarella.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB75"/>
+  <dimension ref="A1:AB100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -826,10 +826,10 @@
       </c>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="n">
-        <v>1020</v>
+        <v>360</v>
       </c>
       <c r="R4" t="n">
-        <v>288</v>
+        <v>360</v>
       </c>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
@@ -922,10 +922,10 @@
       </c>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="n">
-        <v>1020</v>
+        <v>540</v>
       </c>
       <c r="R5" t="n">
-        <v>360</v>
+        <v>540</v>
       </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
@@ -960,7 +960,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Моцарелла без лактозы для сэндвичей "Unagrande", 45%, 0,28 кг, т/ф</t>
+          <t>Моцарелла без лактозы для сэндвичей "Unagrande", 45%, 0,28 кг, т/ф (8 шт)</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -1403,7 +1403,7 @@
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="n">
-        <v>518</v>
+        <v>777</v>
       </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
@@ -1499,7 +1499,7 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="n">
-        <v>518</v>
+        <v>777</v>
       </c>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
@@ -1595,7 +1595,7 @@
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="n">
-        <v>518</v>
+        <v>777</v>
       </c>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
@@ -1978,7 +1978,7 @@
       </c>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="n">
-        <v>1020</v>
+        <v>288</v>
       </c>
       <c r="R16" t="n">
         <v>288</v>
@@ -2267,7 +2267,7 @@
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
       <c r="R19" t="n">
-        <v>518</v>
+        <v>777</v>
       </c>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
@@ -2755,13 +2755,13 @@
         <v>120</v>
       </c>
       <c r="V24" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="W24" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X24" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="Y24" t="n">
         <v>15</v>
@@ -2843,7 +2843,7 @@
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="n">
-        <v>518</v>
+        <v>777</v>
       </c>
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
@@ -2947,13 +2947,13 @@
         <v>120</v>
       </c>
       <c r="V26" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="W26" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X26" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="Y26" t="n">
         <v>15</v>
@@ -3043,13 +3043,13 @@
         <v>120</v>
       </c>
       <c r="V27" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="W27" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X27" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="Y27" t="n">
         <v>15</v>
@@ -3139,13 +3139,13 @@
         <v>120</v>
       </c>
       <c r="V28" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="W28" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X28" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="Y28" t="n">
         <v>15</v>
@@ -3331,13 +3331,13 @@
         <v>120</v>
       </c>
       <c r="V30" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="W30" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X30" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="Y30" t="n">
         <v>15</v>
@@ -3419,7 +3419,7 @@
       <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="n">
-        <v>518</v>
+        <v>540</v>
       </c>
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr"/>
@@ -3456,11 +3456,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Моцарелла Фиор Ди Латте в воде "Unagrande", 50%, 0,125/0,225 кг, ф/п, (8 шт)</t>
+          <t>Моцарелла в воде Фиор Ди Латте "Unagrande", 50%, 0,125/0,225 кг, ф/п, (8 шт)</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Альче</t>
+          <t>Biotec</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -3515,7 +3515,7 @@
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="n">
-        <v>960</v>
+        <v>1200</v>
       </c>
       <c r="S32" t="n">
         <v>25</v>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="U32" t="inlineStr"/>
       <c r="V32" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="W32" t="n">
         <v>25</v>
@@ -3554,11 +3554,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Моцарелла Фиор Ди Латте в воде без лактозы “Unagrande", 45%, 0,125/0,225 кг, ф/п, (8 шт)</t>
+          <t>Моцарелла в воде Фиор Ди Латте без лактозы “Unagrande", 45%, 0,125/0,225 кг, ф/п (8 шт)</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -3577,7 +3577,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Альче</t>
+          <t>Biotec</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -3613,7 +3613,7 @@
       <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="n">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="S33" t="n">
         <v>25</v>
@@ -3623,10 +3623,10 @@
       </c>
       <c r="U33" t="inlineStr"/>
       <c r="V33" t="n">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="W33" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="X33" t="n">
         <v>30</v>
@@ -3656,7 +3656,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -3711,7 +3711,7 @@
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="n">
-        <v>960</v>
+        <v>1200</v>
       </c>
       <c r="S34" t="n">
         <v>25</v>
@@ -3721,7 +3721,7 @@
       </c>
       <c r="U34" t="inlineStr"/>
       <c r="V34" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W34" t="n">
         <v>20</v>
@@ -3754,7 +3754,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -3819,7 +3819,7 @@
       </c>
       <c r="U35" t="inlineStr"/>
       <c r="V35" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W35" t="n">
         <v>20</v>
@@ -3852,7 +3852,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="U36" t="inlineStr"/>
       <c r="V36" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W36" t="n">
         <v>20</v>
@@ -3950,7 +3950,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -4015,7 +4015,7 @@
       </c>
       <c r="U37" t="inlineStr"/>
       <c r="V37" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W37" t="n">
         <v>20</v>
@@ -4048,7 +4048,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -4079,7 +4079,7 @@
         <v>100</v>
       </c>
       <c r="J38" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K38" t="n">
         <v>100</v>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="U38" t="inlineStr"/>
       <c r="V38" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W38" t="n">
         <v>20</v>
@@ -4146,7 +4146,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="U39" t="inlineStr"/>
       <c r="V39" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W39" t="n">
         <v>20</v>
@@ -4244,7 +4244,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -4309,7 +4309,7 @@
       </c>
       <c r="U40" t="inlineStr"/>
       <c r="V40" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W40" t="n">
         <v>20</v>
@@ -4342,7 +4342,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -4361,7 +4361,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Альче</t>
+          <t>Biotec</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -4407,10 +4407,10 @@
       </c>
       <c r="U41" t="inlineStr"/>
       <c r="V41" t="n">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="W41" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="X41" t="n">
         <v>30</v>
@@ -4440,7 +4440,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -4459,7 +4459,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Альче</t>
+          <t>Biotec</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -4505,10 +4505,10 @@
       </c>
       <c r="U42" t="inlineStr"/>
       <c r="V42" t="n">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="W42" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="X42" t="n">
         <v>30</v>
@@ -4534,11 +4534,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Моцарелла Грандиоза в воде "Unagrande", 50%, 0,2/0,36 кг, ф/п</t>
+          <t>Моцарелла в воде Грандиоза "Unagrande", 50%, 0,2/0,36 кг, ф/п</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Альче</t>
+          <t>Biotec</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -4593,7 +4593,7 @@
       <c r="P43" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="n">
-        <v>840</v>
+        <v>120</v>
       </c>
       <c r="S43" t="n">
         <v>25</v>
@@ -4603,7 +4603,7 @@
       </c>
       <c r="U43" t="inlineStr"/>
       <c r="V43" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="W43" t="n">
         <v>25</v>
@@ -4636,7 +4636,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -4655,7 +4655,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Альче</t>
+          <t>Biotec</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -4691,7 +4691,7 @@
       <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="n">
-        <v>876</v>
+        <v>885</v>
       </c>
       <c r="S44" t="n">
         <v>25</v>
@@ -4701,7 +4701,7 @@
       </c>
       <c r="U44" t="inlineStr"/>
       <c r="V44" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="W44" t="n">
         <v>25</v>
@@ -4730,11 +4730,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Моцарелла Чильеджина в воде без лактозы "Unagrande", 45%, 0,125/0,225 кг, ф/п</t>
+          <t>Моцарелла в воде Чильеджина без лактозы "Unagrande", 45%, 0,125/0,225 кг, ф/п (8 шт)</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Альче</t>
+          <t>Biotec</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -4789,7 +4789,7 @@
       <c r="P45" t="inlineStr"/>
       <c r="Q45" t="inlineStr"/>
       <c r="R45" t="n">
-        <v>876</v>
+        <v>885</v>
       </c>
       <c r="S45" t="n">
         <v>25</v>
@@ -4799,10 +4799,10 @@
       </c>
       <c r="U45" t="inlineStr"/>
       <c r="V45" t="n">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="W45" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="X45" t="n">
         <v>30</v>
@@ -4832,7 +4832,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -4887,7 +4887,7 @@
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="n">
-        <v>720</v>
+        <v>708</v>
       </c>
       <c r="S46" t="n">
         <v>25</v>
@@ -4897,7 +4897,7 @@
       </c>
       <c r="U46" t="inlineStr"/>
       <c r="V46" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W46" t="n">
         <v>20</v>
@@ -4930,7 +4930,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -4961,7 +4961,7 @@
         <v>100</v>
       </c>
       <c r="J47" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K47" t="n">
         <v>8</v>
@@ -4985,7 +4985,7 @@
       <c r="P47" t="inlineStr"/>
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="n">
-        <v>720</v>
+        <v>708</v>
       </c>
       <c r="S47" t="n">
         <v>25</v>
@@ -4995,7 +4995,7 @@
       </c>
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W47" t="n">
         <v>20</v>
@@ -5028,7 +5028,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -5083,7 +5083,7 @@
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="n">
-        <v>720</v>
+        <v>708</v>
       </c>
       <c r="S48" t="n">
         <v>25</v>
@@ -5093,7 +5093,7 @@
       </c>
       <c r="U48" t="inlineStr"/>
       <c r="V48" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W48" t="n">
         <v>20</v>
@@ -5126,7 +5126,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -5145,7 +5145,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Альче</t>
+          <t>Biotec</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -5181,7 +5181,7 @@
       <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="n">
-        <v>876</v>
+        <v>885</v>
       </c>
       <c r="S49" t="n">
         <v>25</v>
@@ -5191,10 +5191,10 @@
       </c>
       <c r="U49" t="inlineStr"/>
       <c r="V49" t="n">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="W49" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="X49" t="n">
         <v>30</v>
@@ -5224,7 +5224,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -5279,7 +5279,7 @@
       <c r="P50" t="inlineStr"/>
       <c r="Q50" t="inlineStr"/>
       <c r="R50" t="n">
-        <v>720</v>
+        <v>708</v>
       </c>
       <c r="S50" t="n">
         <v>25</v>
@@ -5289,7 +5289,7 @@
       </c>
       <c r="U50" t="inlineStr"/>
       <c r="V50" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W50" t="n">
         <v>20</v>
@@ -5322,7 +5322,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -5377,7 +5377,7 @@
       <c r="P51" t="inlineStr"/>
       <c r="Q51" t="inlineStr"/>
       <c r="R51" t="n">
-        <v>876</v>
+        <v>885</v>
       </c>
       <c r="S51" t="n">
         <v>25</v>
@@ -5387,7 +5387,7 @@
       </c>
       <c r="U51" t="inlineStr"/>
       <c r="V51" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W51" t="n">
         <v>20</v>
@@ -5612,7 +5612,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -5667,7 +5667,7 @@
       <c r="P54" t="inlineStr"/>
       <c r="Q54" t="inlineStr"/>
       <c r="R54" t="n">
-        <v>960</v>
+        <v>1200</v>
       </c>
       <c r="S54" t="n">
         <v>25</v>
@@ -5677,7 +5677,7 @@
       </c>
       <c r="U54" t="inlineStr"/>
       <c r="V54" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W54" t="n">
         <v>20</v>
@@ -5710,7 +5710,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -5765,7 +5765,7 @@
       <c r="P55" t="inlineStr"/>
       <c r="Q55" t="inlineStr"/>
       <c r="R55" t="n">
-        <v>1020</v>
+        <v>885</v>
       </c>
       <c r="S55" t="n">
         <v>25</v>
@@ -5775,7 +5775,7 @@
       </c>
       <c r="U55" t="inlineStr"/>
       <c r="V55" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W55" t="n">
         <v>20</v>
@@ -5967,13 +5967,13 @@
         <v>120</v>
       </c>
       <c r="V57" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="W57" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X57" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="Y57" t="n">
         <v>15</v>
@@ -6055,7 +6055,7 @@
       <c r="P58" t="inlineStr"/>
       <c r="Q58" t="inlineStr"/>
       <c r="R58" t="n">
-        <v>420</v>
+        <v>540</v>
       </c>
       <c r="S58" t="inlineStr"/>
       <c r="T58" t="inlineStr"/>
@@ -6151,7 +6151,7 @@
       <c r="P59" t="inlineStr"/>
       <c r="Q59" t="inlineStr"/>
       <c r="R59" t="n">
-        <v>432</v>
+        <v>540</v>
       </c>
       <c r="S59" t="inlineStr"/>
       <c r="T59" t="inlineStr"/>
@@ -6284,11 +6284,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Моцарелла Фиор Ди Латте в воде "Pretto", 45%, 1/1,6 кг, ф/п</t>
+          <t>Моцарелла в воде Фиор Ди Латте "Pretto", 45%, 1/1,6 кг, ф/п</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -6342,10 +6342,10 @@
       </c>
       <c r="P61" t="inlineStr"/>
       <c r="Q61" t="n">
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="R61" t="n">
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="S61" t="n">
         <v>25</v>
@@ -6355,7 +6355,7 @@
       </c>
       <c r="U61" t="inlineStr"/>
       <c r="V61" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W61" t="n">
         <v>20</v>
@@ -6384,11 +6384,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Моцарелла Чильеджина в воде "Pretto", 45%, 1/1,8 кг, ф/п</t>
+          <t>Моцарелла в воде Чильеджина "Pretto", 45%, 1/1,6 кг, ф/п</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -6442,10 +6442,10 @@
       </c>
       <c r="P62" t="inlineStr"/>
       <c r="Q62" t="n">
-        <v>702</v>
+        <v>480</v>
       </c>
       <c r="R62" t="n">
-        <v>702</v>
+        <v>480</v>
       </c>
       <c r="S62" t="n">
         <v>25</v>
@@ -6455,7 +6455,7 @@
       </c>
       <c r="U62" t="inlineStr"/>
       <c r="V62" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W62" t="n">
         <v>20</v>
@@ -6586,7 +6586,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -6641,7 +6641,7 @@
       <c r="P64" t="inlineStr"/>
       <c r="Q64" t="inlineStr"/>
       <c r="R64" t="n">
-        <v>720</v>
+        <v>708</v>
       </c>
       <c r="S64" t="n">
         <v>25</v>
@@ -6651,7 +6651,7 @@
       </c>
       <c r="U64" t="inlineStr"/>
       <c r="V64" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W64" t="n">
         <v>20</v>
@@ -6837,7 +6837,7 @@
       <c r="P66" t="inlineStr"/>
       <c r="Q66" t="inlineStr"/>
       <c r="R66" t="n">
-        <v>518</v>
+        <v>540</v>
       </c>
       <c r="S66" t="inlineStr"/>
       <c r="T66" t="inlineStr"/>
@@ -6974,7 +6974,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -7039,7 +7039,7 @@
       </c>
       <c r="U68" t="inlineStr"/>
       <c r="V68" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W68" t="n">
         <v>20</v>
@@ -7072,7 +7072,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -7127,7 +7127,7 @@
       <c r="P69" t="inlineStr"/>
       <c r="Q69" t="inlineStr"/>
       <c r="R69" t="n">
-        <v>720</v>
+        <v>708</v>
       </c>
       <c r="S69" t="n">
         <v>25</v>
@@ -7137,7 +7137,7 @@
       </c>
       <c r="U69" t="inlineStr"/>
       <c r="V69" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W69" t="n">
         <v>20</v>
@@ -7321,7 +7321,7 @@
       <c r="P71" t="inlineStr"/>
       <c r="Q71" t="inlineStr"/>
       <c r="R71" t="n">
-        <v>518</v>
+        <v>777</v>
       </c>
       <c r="S71" t="inlineStr"/>
       <c r="T71" t="inlineStr"/>
@@ -7417,7 +7417,7 @@
       <c r="P72" t="inlineStr"/>
       <c r="Q72" t="inlineStr"/>
       <c r="R72" t="n">
-        <v>518</v>
+        <v>777</v>
       </c>
       <c r="S72" t="inlineStr"/>
       <c r="T72" t="inlineStr"/>
@@ -7458,7 +7458,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -7477,7 +7477,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Альче</t>
+          <t>Biotec</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
@@ -7513,7 +7513,7 @@
       <c r="P73" t="inlineStr"/>
       <c r="Q73" t="inlineStr"/>
       <c r="R73" t="n">
-        <v>960</v>
+        <v>1200</v>
       </c>
       <c r="S73" t="n">
         <v>25</v>
@@ -7523,7 +7523,7 @@
       </c>
       <c r="U73" t="inlineStr"/>
       <c r="V73" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="W73" t="n">
         <v>25</v>
@@ -7707,7 +7707,7 @@
       <c r="P75" t="inlineStr"/>
       <c r="Q75" t="inlineStr"/>
       <c r="R75" t="n">
-        <v>1020</v>
+        <v>360</v>
       </c>
       <c r="S75" t="inlineStr"/>
       <c r="T75" t="inlineStr"/>
@@ -7735,6 +7735,2474 @@
       <c r="AB75" t="inlineStr">
         <is>
           <t>00-00006397</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Моцарелла в воде Фиор Ди Латте "Turatti", 45%, 0,125/0,225 кг, ф/п</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Фиор Ди Латте</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Вода</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Сакко</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Turatti</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>125</v>
+      </c>
+      <c r="J76" t="n">
+        <v>8</v>
+      </c>
+      <c r="K76" t="n">
+        <v>125</v>
+      </c>
+      <c r="L76" t="n">
+        <v>1050</v>
+      </c>
+      <c r="M76" t="n">
+        <v>31</v>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>Мультиголова</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr"/>
+      <c r="Q76" t="n">
+        <v>1200</v>
+      </c>
+      <c r="R76" t="n">
+        <v>1200</v>
+      </c>
+      <c r="S76" t="n">
+        <v>25</v>
+      </c>
+      <c r="T76" t="n">
+        <v>50</v>
+      </c>
+      <c r="U76" t="inlineStr"/>
+      <c r="V76" t="n">
+        <v>35</v>
+      </c>
+      <c r="W76" t="n">
+        <v>20</v>
+      </c>
+      <c r="X76" t="n">
+        <v>35</v>
+      </c>
+      <c r="Y76" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z76" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA76" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB76" t="inlineStr">
+        <is>
+          <t>00-00007161</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Моцарелла в воде Чильеджина "Turatti", 45%, 0,1/0,18 кг, ф/п</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Чильеджина</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Вода</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Сакко</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Turatti</t>
+        </is>
+      </c>
+      <c r="I77" t="n">
+        <v>100</v>
+      </c>
+      <c r="J77" t="n">
+        <v>8</v>
+      </c>
+      <c r="K77" t="n">
+        <v>8</v>
+      </c>
+      <c r="L77" t="n">
+        <v>1050</v>
+      </c>
+      <c r="M77" t="n">
+        <v>31</v>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>Мультиголова</t>
+        </is>
+      </c>
+      <c r="P77" t="inlineStr"/>
+      <c r="Q77" t="n">
+        <v>885</v>
+      </c>
+      <c r="R77" t="n">
+        <v>885</v>
+      </c>
+      <c r="S77" t="n">
+        <v>25</v>
+      </c>
+      <c r="T77" t="n">
+        <v>20</v>
+      </c>
+      <c r="U77" t="inlineStr"/>
+      <c r="V77" t="n">
+        <v>35</v>
+      </c>
+      <c r="W77" t="n">
+        <v>20</v>
+      </c>
+      <c r="X77" t="n">
+        <v>35</v>
+      </c>
+      <c r="Y77" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z77" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA77" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB77" t="inlineStr">
+        <is>
+          <t>00-00007188</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Моцарелла в воде Грандиоза "Unagrande", 45%, 0,2/0,36 кг, ф/п</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Фиор Ди Латте</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Вода</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Biotec</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Unagrande</t>
+        </is>
+      </c>
+      <c r="I78" t="n">
+        <v>200</v>
+      </c>
+      <c r="J78" t="n">
+        <v>8</v>
+      </c>
+      <c r="K78" t="n">
+        <v>200</v>
+      </c>
+      <c r="L78" t="n">
+        <v>1050</v>
+      </c>
+      <c r="M78" t="n">
+        <v>31</v>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>малый Комет</t>
+        </is>
+      </c>
+      <c r="P78" t="inlineStr"/>
+      <c r="Q78" t="n">
+        <v>480</v>
+      </c>
+      <c r="R78" t="n">
+        <v>480</v>
+      </c>
+      <c r="S78" t="n">
+        <v>25</v>
+      </c>
+      <c r="T78" t="n">
+        <v>50</v>
+      </c>
+      <c r="U78" t="inlineStr"/>
+      <c r="V78" t="n">
+        <v>45</v>
+      </c>
+      <c r="W78" t="n">
+        <v>25</v>
+      </c>
+      <c r="X78" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y78" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z78" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA78" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB78" t="inlineStr">
+        <is>
+          <t>00-00008479</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Моцарелла "Unagrande", 45%, 0,5 кг, ф/п (кубики)</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Моцарелла</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Соль</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Альче</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Unagrande</t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>500</v>
+      </c>
+      <c r="J79" t="n">
+        <v>6</v>
+      </c>
+      <c r="K79" t="n">
+        <v>1</v>
+      </c>
+      <c r="L79" t="n">
+        <v>850</v>
+      </c>
+      <c r="M79" t="n">
+        <v>45</v>
+      </c>
+      <c r="N79" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>Мультиголова</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr"/>
+      <c r="Q79" t="n">
+        <v>1200</v>
+      </c>
+      <c r="R79" t="n">
+        <v>1200</v>
+      </c>
+      <c r="S79" t="inlineStr"/>
+      <c r="T79" t="inlineStr"/>
+      <c r="U79" t="inlineStr"/>
+      <c r="V79" t="n">
+        <v>35</v>
+      </c>
+      <c r="W79" t="n">
+        <v>20</v>
+      </c>
+      <c r="X79" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y79" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z79" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA79" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB79" t="inlineStr">
+        <is>
+          <t>00-00008454</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>ОАЭ_Моцарелла в воде Чильеджина без лактозы "Unagrande", 45%, 0,125/0,225 кг, ф/п</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Чильеджина</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Вода</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Альче</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Unagrande</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
+        <v>125</v>
+      </c>
+      <c r="J80" t="n">
+        <v>8</v>
+      </c>
+      <c r="K80" t="n">
+        <v>8</v>
+      </c>
+      <c r="L80" t="n">
+        <v>1050</v>
+      </c>
+      <c r="M80" t="n">
+        <v>31</v>
+      </c>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>Мультиголова</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr"/>
+      <c r="Q80" t="n">
+        <v>876</v>
+      </c>
+      <c r="R80" t="n">
+        <v>876</v>
+      </c>
+      <c r="S80" t="n">
+        <v>25</v>
+      </c>
+      <c r="T80" t="n">
+        <v>20</v>
+      </c>
+      <c r="U80" t="inlineStr"/>
+      <c r="V80" t="n">
+        <v>35</v>
+      </c>
+      <c r="W80" t="n">
+        <v>20</v>
+      </c>
+      <c r="X80" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y80" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z80" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA80" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB80" t="inlineStr">
+        <is>
+          <t>00-00008816</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>ОАЭ_Моцарелла в воде Фиор Ди Латте без лактозы "Unagrande", 45%, 0,125/0,225 кг, ф/п</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Фиор Ди Латте</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Вода</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Альче</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Unagrande</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>125</v>
+      </c>
+      <c r="J81" t="n">
+        <v>8</v>
+      </c>
+      <c r="K81" t="n">
+        <v>125</v>
+      </c>
+      <c r="L81" t="n">
+        <v>1050</v>
+      </c>
+      <c r="M81" t="n">
+        <v>31</v>
+      </c>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Мультиголова</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr"/>
+      <c r="Q81" t="n">
+        <v>1200</v>
+      </c>
+      <c r="R81" t="n">
+        <v>1200</v>
+      </c>
+      <c r="S81" t="n">
+        <v>25</v>
+      </c>
+      <c r="T81" t="n">
+        <v>50</v>
+      </c>
+      <c r="U81" t="inlineStr"/>
+      <c r="V81" t="n">
+        <v>35</v>
+      </c>
+      <c r="W81" t="n">
+        <v>20</v>
+      </c>
+      <c r="X81" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y81" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z81" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA81" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB81" t="inlineStr">
+        <is>
+          <t>00-00008815</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>ОАЭ_Моцарелла для сэндвичей без лактозы "Unagrande", 45%, 0,28 кг, т/ф</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Для пиццы</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Соль</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Альче</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Unagrande</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>280</v>
+      </c>
+      <c r="J82" t="n">
+        <v>8</v>
+      </c>
+      <c r="K82" t="n">
+        <v>280</v>
+      </c>
+      <c r="L82" t="n">
+        <v>850</v>
+      </c>
+      <c r="M82" t="n">
+        <v>65</v>
+      </c>
+      <c r="N82" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Ульма</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr"/>
+      <c r="Q82" t="n">
+        <v>1020</v>
+      </c>
+      <c r="R82" t="n">
+        <v>1020</v>
+      </c>
+      <c r="S82" t="inlineStr"/>
+      <c r="T82" t="inlineStr"/>
+      <c r="U82" t="n">
+        <v>120</v>
+      </c>
+      <c r="V82" t="n">
+        <v>35</v>
+      </c>
+      <c r="W82" t="n">
+        <v>20</v>
+      </c>
+      <c r="X82" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y82" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z82" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA82" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB82" t="inlineStr">
+        <is>
+          <t>00-00008810</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>ОАЭ_Моцарелла без лактозы "Unagrande", 45%, 0,15 (кубики)</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Моцарелла</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Соль</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Альче</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Unagrande</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
+        <v>120</v>
+      </c>
+      <c r="J83" t="n">
+        <v>6</v>
+      </c>
+      <c r="K83" t="n">
+        <v>1</v>
+      </c>
+      <c r="L83" t="n">
+        <v>850</v>
+      </c>
+      <c r="M83" t="n">
+        <v>45</v>
+      </c>
+      <c r="N83" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>Мультиголова</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr"/>
+      <c r="Q83" t="n">
+        <v>360</v>
+      </c>
+      <c r="R83" t="n">
+        <v>360</v>
+      </c>
+      <c r="S83" t="inlineStr"/>
+      <c r="T83" t="inlineStr"/>
+      <c r="U83" t="inlineStr"/>
+      <c r="V83" t="n">
+        <v>35</v>
+      </c>
+      <c r="W83" t="n">
+        <v>20</v>
+      </c>
+      <c r="X83" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y83" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z83" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA83" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB83" t="inlineStr">
+        <is>
+          <t>00-00008814</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>ОАЭ_Моцарелла палочки без лактозы "Unagrande", 45%, 0,12 кг, т/ф</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Для пиццы</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Соль</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Альче</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Unagrande</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>120</v>
+      </c>
+      <c r="J84" t="n">
+        <v>10</v>
+      </c>
+      <c r="K84" t="n">
+        <v>30</v>
+      </c>
+      <c r="L84" t="n">
+        <v>850</v>
+      </c>
+      <c r="M84" t="n">
+        <v>65</v>
+      </c>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Ульма</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr"/>
+      <c r="Q84" t="n">
+        <v>777</v>
+      </c>
+      <c r="R84" t="n">
+        <v>777</v>
+      </c>
+      <c r="S84" t="inlineStr"/>
+      <c r="T84" t="inlineStr"/>
+      <c r="U84" t="n">
+        <v>10</v>
+      </c>
+      <c r="V84" t="n">
+        <v>35</v>
+      </c>
+      <c r="W84" t="n">
+        <v>20</v>
+      </c>
+      <c r="X84" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y84" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z84" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA84" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB84" t="inlineStr">
+        <is>
+          <t>00-00008811</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Сулугуни палочки без лактозы "Умалат", 45%, 0,12 кг, т/ф</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Сулугуни</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Соль</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Альче</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Умалат</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>120</v>
+      </c>
+      <c r="J85" t="n">
+        <v>6</v>
+      </c>
+      <c r="K85" t="n">
+        <v>30</v>
+      </c>
+      <c r="L85" t="n">
+        <v>850</v>
+      </c>
+      <c r="M85" t="n">
+        <v>50</v>
+      </c>
+      <c r="N85" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>Ульма</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr"/>
+      <c r="Q85" t="n">
+        <v>777</v>
+      </c>
+      <c r="R85" t="n">
+        <v>777</v>
+      </c>
+      <c r="S85" t="inlineStr"/>
+      <c r="T85" t="inlineStr"/>
+      <c r="U85" t="n">
+        <v>10</v>
+      </c>
+      <c r="V85" t="n">
+        <v>40</v>
+      </c>
+      <c r="W85" t="n">
+        <v>20</v>
+      </c>
+      <c r="X85" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y85" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z85" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA85" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB85" t="inlineStr">
+        <is>
+          <t>00-00008879</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Моцарелла в воде Чильеджина "Unagrande", 45%, 0,125/0,225 кг, ф/п</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Чильеджина</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Вода</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Biotec</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Unagrande</t>
+        </is>
+      </c>
+      <c r="I86" t="n">
+        <v>125</v>
+      </c>
+      <c r="J86" t="n">
+        <v>8</v>
+      </c>
+      <c r="K86" t="n">
+        <v>8</v>
+      </c>
+      <c r="L86" t="n">
+        <v>1050</v>
+      </c>
+      <c r="M86" t="n">
+        <v>25</v>
+      </c>
+      <c r="N86" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>Мультиголова</t>
+        </is>
+      </c>
+      <c r="P86" t="inlineStr"/>
+      <c r="Q86" t="n">
+        <v>885</v>
+      </c>
+      <c r="R86" t="n">
+        <v>885</v>
+      </c>
+      <c r="S86" t="n">
+        <v>25</v>
+      </c>
+      <c r="T86" t="n">
+        <v>20</v>
+      </c>
+      <c r="U86" t="inlineStr"/>
+      <c r="V86" t="n">
+        <v>45</v>
+      </c>
+      <c r="W86" t="n">
+        <v>25</v>
+      </c>
+      <c r="X86" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y86" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z86" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA86" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB86" t="inlineStr">
+        <is>
+          <t>00-00008507</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Моцарелла в воде Фиор Ди Латте "Unagrande", 45%, 0,125/0,225 кг, ф/п</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Фиор Ди Латте</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Вода</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Biotec</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Unagrande</t>
+        </is>
+      </c>
+      <c r="I87" t="n">
+        <v>125</v>
+      </c>
+      <c r="J87" t="n">
+        <v>8</v>
+      </c>
+      <c r="K87" t="n">
+        <v>125</v>
+      </c>
+      <c r="L87" t="n">
+        <v>1050</v>
+      </c>
+      <c r="M87" t="n">
+        <v>31</v>
+      </c>
+      <c r="N87" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>Мультиголова</t>
+        </is>
+      </c>
+      <c r="P87" t="inlineStr"/>
+      <c r="Q87" t="n">
+        <v>1200</v>
+      </c>
+      <c r="R87" t="n">
+        <v>1200</v>
+      </c>
+      <c r="S87" t="n">
+        <v>25</v>
+      </c>
+      <c r="T87" t="n">
+        <v>50</v>
+      </c>
+      <c r="U87" t="inlineStr"/>
+      <c r="V87" t="n">
+        <v>45</v>
+      </c>
+      <c r="W87" t="n">
+        <v>25</v>
+      </c>
+      <c r="X87" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y87" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z87" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA87" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB87" t="inlineStr">
+        <is>
+          <t>00-00008508</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Моцарелла для бутербродов «Вкусвилл», 45%, 0,2 кг т/ф</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Для пиццы</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Соль</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Сакко</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Вкусвилл</t>
+        </is>
+      </c>
+      <c r="I88" t="n">
+        <v>200</v>
+      </c>
+      <c r="J88" t="n">
+        <v>9</v>
+      </c>
+      <c r="K88" t="n">
+        <v>200</v>
+      </c>
+      <c r="L88" t="n">
+        <v>850</v>
+      </c>
+      <c r="M88" t="n">
+        <v>1020</v>
+      </c>
+      <c r="N88" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>Ульма</t>
+        </is>
+      </c>
+      <c r="P88" t="inlineStr"/>
+      <c r="Q88" t="n">
+        <v>1020</v>
+      </c>
+      <c r="R88" t="n">
+        <v>1020</v>
+      </c>
+      <c r="S88" t="inlineStr"/>
+      <c r="T88" t="inlineStr"/>
+      <c r="U88" t="n">
+        <v>90</v>
+      </c>
+      <c r="V88" t="n">
+        <v>40</v>
+      </c>
+      <c r="W88" t="n">
+        <v>20</v>
+      </c>
+      <c r="X88" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y88" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z88" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA88" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB88" t="inlineStr">
+        <is>
+          <t>00-00008894</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Сулугуни "Foodfest", 45%, 0,37 кг, т/ф</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Сулугуни</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Соль</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Альче</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Foodfest</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
+        <v>370</v>
+      </c>
+      <c r="J89" t="n">
+        <v>6</v>
+      </c>
+      <c r="K89" t="n">
+        <v>370</v>
+      </c>
+      <c r="L89" t="n">
+        <v>850</v>
+      </c>
+      <c r="M89" t="n">
+        <v>50</v>
+      </c>
+      <c r="N89" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>Ульма</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr"/>
+      <c r="Q89" t="n">
+        <v>1020</v>
+      </c>
+      <c r="R89" t="n">
+        <v>1020</v>
+      </c>
+      <c r="S89" t="inlineStr"/>
+      <c r="T89" t="inlineStr"/>
+      <c r="U89" t="n">
+        <v>120</v>
+      </c>
+      <c r="V89" t="n">
+        <v>35</v>
+      </c>
+      <c r="W89" t="n">
+        <v>20</v>
+      </c>
+      <c r="X89" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y89" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z89" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA89" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB89" t="inlineStr">
+        <is>
+          <t>00-00008525</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Сулугуни палочки "Умалат", 45%, 3,5 кг, п/л</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Сулугуни</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Соль</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Альче</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Умалат</t>
+        </is>
+      </c>
+      <c r="I90" t="n">
+        <v>3500</v>
+      </c>
+      <c r="J90" t="n">
+        <v>8</v>
+      </c>
+      <c r="K90" t="n">
+        <v>30</v>
+      </c>
+      <c r="L90" t="n">
+        <v>850</v>
+      </c>
+      <c r="M90" t="n">
+        <v>50</v>
+      </c>
+      <c r="N90" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>Ульма</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr"/>
+      <c r="Q90" t="n">
+        <v>540</v>
+      </c>
+      <c r="R90" t="n">
+        <v>540</v>
+      </c>
+      <c r="S90" t="inlineStr"/>
+      <c r="T90" t="inlineStr"/>
+      <c r="U90" t="n">
+        <v>10</v>
+      </c>
+      <c r="V90" t="n">
+        <v>35</v>
+      </c>
+      <c r="W90" t="n">
+        <v>20</v>
+      </c>
+      <c r="X90" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y90" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z90" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA90" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB90" t="inlineStr">
+        <is>
+          <t>00-00008988</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Моцарелла в воде Чильеджина без лактозы "Unagrande", 45%, 0,125/0,225 кг, ф/п (6 шт)</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Чильеджина</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Вода</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Biotec</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Unagrande</t>
+        </is>
+      </c>
+      <c r="I91" t="n">
+        <v>125</v>
+      </c>
+      <c r="J91" t="n">
+        <v>6</v>
+      </c>
+      <c r="K91" t="n">
+        <v>8</v>
+      </c>
+      <c r="L91" t="n">
+        <v>1050</v>
+      </c>
+      <c r="M91" t="n">
+        <v>31</v>
+      </c>
+      <c r="N91" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>Мультиголова</t>
+        </is>
+      </c>
+      <c r="P91" t="inlineStr"/>
+      <c r="Q91" t="n">
+        <v>876</v>
+      </c>
+      <c r="R91" t="n">
+        <v>876</v>
+      </c>
+      <c r="S91" t="n">
+        <v>25</v>
+      </c>
+      <c r="T91" t="n">
+        <v>20</v>
+      </c>
+      <c r="U91" t="inlineStr"/>
+      <c r="V91" t="n">
+        <v>35</v>
+      </c>
+      <c r="W91" t="n">
+        <v>25</v>
+      </c>
+      <c r="X91" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y91" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z91" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA91" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB91" t="inlineStr">
+        <is>
+          <t>00-00009215</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Моцарелла в воде Фиор Ди Латте без лактозы “Unagrande", 45%, 0,125/0,225 кг, ф/п (6 шт)</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Фиор Ди Латте</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Вода</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Biotec</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Unagrande</t>
+        </is>
+      </c>
+      <c r="I92" t="n">
+        <v>125</v>
+      </c>
+      <c r="J92" t="n">
+        <v>6</v>
+      </c>
+      <c r="K92" t="n">
+        <v>125</v>
+      </c>
+      <c r="L92" t="n">
+        <v>1050</v>
+      </c>
+      <c r="M92" t="n">
+        <v>25</v>
+      </c>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>Мультиголова</t>
+        </is>
+      </c>
+      <c r="P92" t="inlineStr"/>
+      <c r="Q92" t="n">
+        <v>1200</v>
+      </c>
+      <c r="R92" t="n">
+        <v>1200</v>
+      </c>
+      <c r="S92" t="n">
+        <v>25</v>
+      </c>
+      <c r="T92" t="n">
+        <v>50</v>
+      </c>
+      <c r="U92" t="inlineStr"/>
+      <c r="V92" t="n">
+        <v>35</v>
+      </c>
+      <c r="W92" t="n">
+        <v>25</v>
+      </c>
+      <c r="X92" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y92" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z92" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA92" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB92" t="inlineStr">
+        <is>
+          <t>00-00009216</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Моцарелла без лактозы для сэндвичей "Unagrande", 45%, 0,28 кг, т/ф (6 шт)</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Для пиццы</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Соль</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Альче</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Unagrande</t>
+        </is>
+      </c>
+      <c r="I93" t="n">
+        <v>280</v>
+      </c>
+      <c r="J93" t="n">
+        <v>8</v>
+      </c>
+      <c r="K93" t="n">
+        <v>280</v>
+      </c>
+      <c r="L93" t="n">
+        <v>850</v>
+      </c>
+      <c r="M93" t="n">
+        <v>65</v>
+      </c>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>Ульма</t>
+        </is>
+      </c>
+      <c r="P93" t="inlineStr"/>
+      <c r="Q93" t="n">
+        <v>1020</v>
+      </c>
+      <c r="R93" t="n">
+        <v>1020</v>
+      </c>
+      <c r="S93" t="inlineStr"/>
+      <c r="T93" t="inlineStr"/>
+      <c r="U93" t="n">
+        <v>120</v>
+      </c>
+      <c r="V93" t="n">
+        <v>40</v>
+      </c>
+      <c r="W93" t="n">
+        <v>20</v>
+      </c>
+      <c r="X93" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y93" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z93" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA93" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB93" t="inlineStr">
+        <is>
+          <t>00-00009217</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Моцарелла для пиццы "SORIMA" 45%, 1,2 кг, т/ф</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Для пиццы</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Соль</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Альче</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>SORIMA</t>
+        </is>
+      </c>
+      <c r="I94" t="n">
+        <v>1200</v>
+      </c>
+      <c r="J94" t="n">
+        <v>8</v>
+      </c>
+      <c r="K94" t="n">
+        <v>1200</v>
+      </c>
+      <c r="L94" t="n">
+        <v>850</v>
+      </c>
+      <c r="M94" t="n">
+        <v>65</v>
+      </c>
+      <c r="N94" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>Ульма</t>
+        </is>
+      </c>
+      <c r="P94" t="inlineStr"/>
+      <c r="Q94" t="n">
+        <v>1020</v>
+      </c>
+      <c r="R94" t="n">
+        <v>1020</v>
+      </c>
+      <c r="S94" t="inlineStr"/>
+      <c r="T94" t="inlineStr"/>
+      <c r="U94" t="n">
+        <v>120</v>
+      </c>
+      <c r="V94" t="n">
+        <v>35</v>
+      </c>
+      <c r="W94" t="n">
+        <v>20</v>
+      </c>
+      <c r="X94" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y94" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z94" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA94" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB94" t="inlineStr">
+        <is>
+          <t>00-00009233</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Моцарелла в воде Чильеджина «SPAR», 45%, 0,1/0,18 кг, ф/п  </t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Чильеджина</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Вода</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Сакко</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>SPAR</t>
+        </is>
+      </c>
+      <c r="I95" t="n">
+        <v>100</v>
+      </c>
+      <c r="J95" t="n">
+        <v>8</v>
+      </c>
+      <c r="K95" t="n">
+        <v>8</v>
+      </c>
+      <c r="L95" t="n">
+        <v>1050</v>
+      </c>
+      <c r="M95" t="n">
+        <v>31</v>
+      </c>
+      <c r="N95" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>Мультиголова</t>
+        </is>
+      </c>
+      <c r="P95" t="inlineStr"/>
+      <c r="Q95" t="n">
+        <v>708</v>
+      </c>
+      <c r="R95" t="n">
+        <v>708</v>
+      </c>
+      <c r="S95" t="n">
+        <v>25</v>
+      </c>
+      <c r="T95" t="n">
+        <v>20</v>
+      </c>
+      <c r="U95" t="inlineStr"/>
+      <c r="V95" t="n">
+        <v>35</v>
+      </c>
+      <c r="W95" t="n">
+        <v>20</v>
+      </c>
+      <c r="X95" t="n">
+        <v>35</v>
+      </c>
+      <c r="Y95" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z95" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA95" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB95" t="inlineStr">
+        <is>
+          <t>00-00009632</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Моцарелла в воде Фиор Ди Латте «SPAR», 45%, 0,1/0,18 кг, ф/п</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Фиор Ди Латте</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Вода</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Сакко</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>SPAR</t>
+        </is>
+      </c>
+      <c r="I96" t="n">
+        <v>100</v>
+      </c>
+      <c r="J96" t="n">
+        <v>8</v>
+      </c>
+      <c r="K96" t="n">
+        <v>100</v>
+      </c>
+      <c r="L96" t="n">
+        <v>1050</v>
+      </c>
+      <c r="M96" t="n">
+        <v>31</v>
+      </c>
+      <c r="N96" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>Мультиголова</t>
+        </is>
+      </c>
+      <c r="P96" t="inlineStr"/>
+      <c r="Q96" t="n">
+        <v>960</v>
+      </c>
+      <c r="R96" t="n">
+        <v>960</v>
+      </c>
+      <c r="S96" t="n">
+        <v>25</v>
+      </c>
+      <c r="T96" t="n">
+        <v>50</v>
+      </c>
+      <c r="U96" t="inlineStr"/>
+      <c r="V96" t="n">
+        <v>35</v>
+      </c>
+      <c r="W96" t="n">
+        <v>20</v>
+      </c>
+      <c r="X96" t="n">
+        <v>35</v>
+      </c>
+      <c r="Y96" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z96" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA96" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB96" t="inlineStr">
+        <is>
+          <t>00-00009633</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Моцарелла "Pretto", 45%, 0,37 кг, т/ф</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Для пиццы</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Соль</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Сакко</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>Фермерская коллекция</t>
+        </is>
+      </c>
+      <c r="I97" t="n">
+        <v>370</v>
+      </c>
+      <c r="J97" t="n">
+        <v>9</v>
+      </c>
+      <c r="K97" t="n">
+        <v>370</v>
+      </c>
+      <c r="L97" t="n">
+        <v>850</v>
+      </c>
+      <c r="M97" t="n">
+        <v>65</v>
+      </c>
+      <c r="N97" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>Ульма</t>
+        </is>
+      </c>
+      <c r="P97" t="inlineStr"/>
+      <c r="Q97" t="n">
+        <v>1020</v>
+      </c>
+      <c r="R97" t="n">
+        <v>1020</v>
+      </c>
+      <c r="S97" t="inlineStr"/>
+      <c r="T97" t="inlineStr"/>
+      <c r="U97" t="n">
+        <v>120</v>
+      </c>
+      <c r="V97" t="n">
+        <v>40</v>
+      </c>
+      <c r="W97" t="n">
+        <v>20</v>
+      </c>
+      <c r="X97" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y97" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z97" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA97" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB97" t="inlineStr">
+        <is>
+          <t>00-00009887</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Моцарелла для пиццы "Aventino", 45%, 0,2 кг, т/ф</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Для пиццы</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Соль</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Сакко</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>Aventino</t>
+        </is>
+      </c>
+      <c r="I98" t="n">
+        <v>200</v>
+      </c>
+      <c r="J98" t="n">
+        <v>9</v>
+      </c>
+      <c r="K98" t="n">
+        <v>200</v>
+      </c>
+      <c r="L98" t="n">
+        <v>850</v>
+      </c>
+      <c r="M98" t="n">
+        <v>65</v>
+      </c>
+      <c r="N98" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>Ульма</t>
+        </is>
+      </c>
+      <c r="P98" t="inlineStr"/>
+      <c r="Q98" t="n">
+        <v>1020</v>
+      </c>
+      <c r="R98" t="n">
+        <v>1020</v>
+      </c>
+      <c r="S98" t="inlineStr"/>
+      <c r="T98" t="inlineStr"/>
+      <c r="U98" t="n">
+        <v>90</v>
+      </c>
+      <c r="V98" t="n">
+        <v>40</v>
+      </c>
+      <c r="W98" t="n">
+        <v>20</v>
+      </c>
+      <c r="X98" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y98" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z98" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA98" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB98" t="inlineStr">
+        <is>
+          <t>00-00010112</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Моцарелла без лактозы «Вкусвилл», 45%, 0,1 кг, ф/п (кубики)</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Для пиццы</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Соль</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Альче</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>Unagrande</t>
+        </is>
+      </c>
+      <c r="I99" t="n">
+        <v>100</v>
+      </c>
+      <c r="J99" t="n">
+        <v>8</v>
+      </c>
+      <c r="K99" t="n">
+        <v>280</v>
+      </c>
+      <c r="L99" t="n">
+        <v>850</v>
+      </c>
+      <c r="M99" t="n">
+        <v>65</v>
+      </c>
+      <c r="N99" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>Ульма</t>
+        </is>
+      </c>
+      <c r="P99" t="inlineStr"/>
+      <c r="Q99" t="n">
+        <v>1020</v>
+      </c>
+      <c r="R99" t="n">
+        <v>1020</v>
+      </c>
+      <c r="S99" t="inlineStr"/>
+      <c r="T99" t="inlineStr"/>
+      <c r="U99" t="n">
+        <v>120</v>
+      </c>
+      <c r="V99" t="n">
+        <v>40</v>
+      </c>
+      <c r="W99" t="n">
+        <v>20</v>
+      </c>
+      <c r="X99" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y99" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z99" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA99" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB99" t="inlineStr">
+        <is>
+          <t>00-00010673</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Моцарелла палочки без лактозы «Вкусвилл», 45%, 0,12 кг, т/ф</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Для пиццы</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Соль</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Альче</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>Вкусвилл</t>
+        </is>
+      </c>
+      <c r="I100" t="n">
+        <v>120</v>
+      </c>
+      <c r="J100" t="n">
+        <v>10</v>
+      </c>
+      <c r="K100" t="n">
+        <v>30</v>
+      </c>
+      <c r="L100" t="n">
+        <v>850</v>
+      </c>
+      <c r="M100" t="n">
+        <v>65</v>
+      </c>
+      <c r="N100" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>Ульма</t>
+        </is>
+      </c>
+      <c r="P100" t="inlineStr"/>
+      <c r="Q100" t="n">
+        <v>777</v>
+      </c>
+      <c r="R100" t="n">
+        <v>777</v>
+      </c>
+      <c r="S100" t="inlineStr"/>
+      <c r="T100" t="inlineStr"/>
+      <c r="U100" t="n">
+        <v>10</v>
+      </c>
+      <c r="V100" t="n">
+        <v>35</v>
+      </c>
+      <c r="W100" t="n">
+        <v>20</v>
+      </c>
+      <c r="X100" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y100" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z100" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA100" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB100" t="inlineStr">
+        <is>
+          <t>00-00010669</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: change db params
</commit_message>
<xml_diff>
--- a/app/data/static/params/mozzarella.xlsx
+++ b/app/data/static/params/mozzarella.xlsx
@@ -951,13 +951,14 @@
   </sheetPr>
   <dimension ref="A1:AC101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AI91" activeCellId="0" sqref="AI91"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AG53" activeCellId="0" sqref="AG52:AG53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="11" min="3" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="11" min="7" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="12" min="12" style="0" width="8.54"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="27" min="13" style="0" width="8.53"/>
   </cols>
   <sheetData>
@@ -3431,7 +3432,7 @@
         <v>5</v>
       </c>
       <c r="AB32" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC32" s="0" t="s">
         <v>118</v>
@@ -3511,7 +3512,7 @@
         <v>5</v>
       </c>
       <c r="AB33" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC33" s="0" t="s">
         <v>120</v>
@@ -3591,7 +3592,7 @@
         <v>5</v>
       </c>
       <c r="AB34" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC34" s="0" t="s">
         <v>122</v>
@@ -3671,7 +3672,7 @@
         <v>5</v>
       </c>
       <c r="AB35" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC35" s="0" t="s">
         <v>124</v>
@@ -3751,7 +3752,7 @@
         <v>5</v>
       </c>
       <c r="AB36" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC36" s="0" t="s">
         <v>126</v>
@@ -3831,7 +3832,7 @@
         <v>5</v>
       </c>
       <c r="AB37" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC37" s="0" t="s">
         <v>128</v>
@@ -3911,7 +3912,7 @@
         <v>5</v>
       </c>
       <c r="AB38" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC38" s="0" t="s">
         <v>131</v>
@@ -3991,7 +3992,7 @@
         <v>5</v>
       </c>
       <c r="AB39" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC39" s="0" t="s">
         <v>134</v>
@@ -4071,7 +4072,7 @@
         <v>5</v>
       </c>
       <c r="AB40" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC40" s="0" t="s">
         <v>137</v>
@@ -4151,7 +4152,7 @@
         <v>5</v>
       </c>
       <c r="AB41" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC41" s="0" t="s">
         <v>139</v>
@@ -4231,7 +4232,7 @@
         <v>5</v>
       </c>
       <c r="AB42" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC42" s="0" t="s">
         <v>141</v>
@@ -4311,7 +4312,7 @@
         <v>5</v>
       </c>
       <c r="AB43" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC43" s="0" t="s">
         <v>144</v>
@@ -4391,7 +4392,7 @@
         <v>5</v>
       </c>
       <c r="AB44" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC44" s="0" t="s">
         <v>147</v>
@@ -4471,7 +4472,7 @@
         <v>5</v>
       </c>
       <c r="AB45" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC45" s="0" t="s">
         <v>149</v>
@@ -4551,7 +4552,7 @@
         <v>5</v>
       </c>
       <c r="AB46" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC46" s="0" t="s">
         <v>151</v>
@@ -4631,7 +4632,7 @@
         <v>5</v>
       </c>
       <c r="AB47" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC47" s="0" t="s">
         <v>153</v>
@@ -4711,7 +4712,7 @@
         <v>5</v>
       </c>
       <c r="AB48" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC48" s="0" t="s">
         <v>155</v>
@@ -4791,7 +4792,7 @@
         <v>5</v>
       </c>
       <c r="AB49" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC49" s="0" t="s">
         <v>157</v>
@@ -4871,7 +4872,7 @@
         <v>5</v>
       </c>
       <c r="AB50" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC50" s="0" t="s">
         <v>159</v>
@@ -4951,7 +4952,7 @@
         <v>5</v>
       </c>
       <c r="AB51" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC51" s="0" t="s">
         <v>161</v>
@@ -5185,7 +5186,7 @@
         <v>5</v>
       </c>
       <c r="AB54" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC54" s="0" t="s">
         <v>167</v>
@@ -5265,7 +5266,7 @@
         <v>5</v>
       </c>
       <c r="AB55" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC55" s="0" t="s">
         <v>169</v>
@@ -5733,7 +5734,7 @@
         <v>5</v>
       </c>
       <c r="AB61" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC61" s="0" t="s">
         <v>181</v>
@@ -5816,7 +5817,7 @@
         <v>5</v>
       </c>
       <c r="AB62" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC62" s="0" t="s">
         <v>183</v>
@@ -5976,7 +5977,7 @@
         <v>5</v>
       </c>
       <c r="AB64" s="0" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC64" s="0" t="s">
         <v>188</v>
@@ -6290,7 +6291,7 @@
         <v>5</v>
       </c>
       <c r="AB68" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC68" s="0" t="s">
         <v>198</v>
@@ -6370,7 +6371,7 @@
         <v>5</v>
       </c>
       <c r="AB69" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC69" s="0" t="s">
         <v>200</v>
@@ -6681,7 +6682,7 @@
         <v>5</v>
       </c>
       <c r="AB73" s="0" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC73" s="0" t="s">
         <v>208</v>
@@ -6918,7 +6919,7 @@
         <v>5</v>
       </c>
       <c r="AB76" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC76" s="0" t="s">
         <v>215</v>
@@ -7001,7 +7002,7 @@
         <v>5</v>
       </c>
       <c r="AB77" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC77" s="0" t="s">
         <v>217</v>
@@ -7084,7 +7085,7 @@
         <v>5</v>
       </c>
       <c r="AB78" s="0" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC78" s="0" t="s">
         <v>219</v>
@@ -7244,7 +7245,7 @@
         <v>5</v>
       </c>
       <c r="AB80" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC80" s="0" t="s">
         <v>223</v>
@@ -7327,7 +7328,7 @@
         <v>5</v>
       </c>
       <c r="AB81" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC81" s="0" t="s">
         <v>225</v>
@@ -7727,7 +7728,7 @@
         <v>5</v>
       </c>
       <c r="AB86" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC86" s="0" t="s">
         <v>235</v>
@@ -7810,7 +7811,7 @@
         <v>5</v>
       </c>
       <c r="AB87" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC87" s="0" t="s">
         <v>237</v>
@@ -8133,7 +8134,7 @@
         <v>5</v>
       </c>
       <c r="AB91" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC91" s="0" t="s">
         <v>246</v>
@@ -8216,7 +8217,7 @@
         <v>5</v>
       </c>
       <c r="AB92" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC92" s="0" t="s">
         <v>248</v>
@@ -8459,7 +8460,7 @@
         <v>5</v>
       </c>
       <c r="AB95" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC95" s="0" t="s">
         <v>256</v>
@@ -8542,7 +8543,7 @@
         <v>5</v>
       </c>
       <c r="AB96" s="2" t="n">
-        <v>1635</v>
+        <v>900</v>
       </c>
       <c r="AC96" s="0" t="s">
         <v>258</v>

</xml_diff>

<commit_message>
Fix: mozzarella db params
</commit_message>
<xml_diff>
--- a/app/data/static/params/mozzarella.xlsx
+++ b/app/data/static/params/mozzarella.xlsx
@@ -804,16 +804,19 @@
   </sheetPr>
   <dimension ref="A1:AC78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V79" activeCellId="0" sqref="V79"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W24" activeCellId="0" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="8"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="12" min="5" style="0" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="0" width="15"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="16" min="14" style="0" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="17" min="17" style="0" width="8"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="21" min="18" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="4.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="8.72"/>
   </cols>
@@ -957,7 +960,7 @@
         <v>90</v>
       </c>
       <c r="V2" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W2" s="0" t="n">
         <v>20</v>
@@ -1034,7 +1037,7 @@
         <v>120</v>
       </c>
       <c r="V3" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W3" s="0" t="n">
         <v>20</v>
@@ -1111,7 +1114,7 @@
         <v>540</v>
       </c>
       <c r="V4" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W4" s="0" t="n">
         <v>20</v>
@@ -1188,7 +1191,7 @@
         <v>90</v>
       </c>
       <c r="V5" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W5" s="0" t="n">
         <v>20</v>
@@ -1265,7 +1268,7 @@
         <v>10</v>
       </c>
       <c r="V6" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W6" s="0" t="n">
         <v>20</v>
@@ -1342,7 +1345,7 @@
         <v>10</v>
       </c>
       <c r="V7" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W7" s="0" t="n">
         <v>20</v>
@@ -1419,7 +1422,7 @@
         <v>10</v>
       </c>
       <c r="V8" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W8" s="0" t="n">
         <v>20</v>
@@ -1496,7 +1499,7 @@
         <v>90</v>
       </c>
       <c r="V9" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W9" s="0" t="n">
         <v>20</v>
@@ -1573,7 +1576,7 @@
         <v>288</v>
       </c>
       <c r="V10" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W10" s="0" t="n">
         <v>20</v>
@@ -1650,7 +1653,7 @@
         <v>90</v>
       </c>
       <c r="V11" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W11" s="0" t="n">
         <v>20</v>
@@ -1727,7 +1730,7 @@
         <v>90</v>
       </c>
       <c r="V12" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W12" s="0" t="n">
         <v>20</v>
@@ -1804,7 +1807,7 @@
         <v>10</v>
       </c>
       <c r="V13" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W13" s="0" t="n">
         <v>20</v>
@@ -1881,7 +1884,7 @@
         <v>90</v>
       </c>
       <c r="V14" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W14" s="0" t="n">
         <v>20</v>
@@ -1958,7 +1961,7 @@
         <v>90</v>
       </c>
       <c r="V15" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W15" s="0" t="n">
         <v>20</v>
@@ -2035,7 +2038,7 @@
         <v>120</v>
       </c>
       <c r="V16" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W16" s="0" t="n">
         <v>20</v>
@@ -2112,7 +2115,7 @@
         <v>10</v>
       </c>
       <c r="V17" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W17" s="0" t="n">
         <v>20</v>
@@ -2290,7 +2293,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
@@ -3754,7 +3757,7 @@
         <v>90</v>
       </c>
       <c r="V37" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W37" s="0" t="n">
         <v>20</v>
@@ -3831,7 +3834,7 @@
         <v>120</v>
       </c>
       <c r="V38" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W38" s="0" t="n">
         <v>20</v>
@@ -4074,7 +4077,7 @@
         <v>90</v>
       </c>
       <c r="V41" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W41" s="0" t="n">
         <v>20</v>
@@ -4151,7 +4154,7 @@
         <v>10</v>
       </c>
       <c r="V42" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W42" s="0" t="n">
         <v>20</v>
@@ -4228,7 +4231,7 @@
         <v>10</v>
       </c>
       <c r="V43" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W43" s="0" t="n">
         <v>20</v>
@@ -4305,7 +4308,7 @@
         <v>120</v>
       </c>
       <c r="V44" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W44" s="0" t="n">
         <v>20</v>
@@ -4720,7 +4723,7 @@
         <v>10</v>
       </c>
       <c r="V49" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W49" s="0" t="n">
         <v>20</v>
@@ -4797,7 +4800,7 @@
         <v>10</v>
       </c>
       <c r="V50" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W50" s="0" t="n">
         <v>20</v>
@@ -4874,7 +4877,7 @@
         <v>90</v>
       </c>
       <c r="V51" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W51" s="0" t="n">
         <v>20</v>
@@ -4948,7 +4951,7 @@
         <v>360</v>
       </c>
       <c r="V52" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W52" s="0" t="n">
         <v>20</v>
@@ -5230,7 +5233,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
@@ -5283,7 +5286,7 @@
         <v>1200</v>
       </c>
       <c r="V56" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W56" s="0" t="n">
         <v>20</v>
@@ -5479,7 +5482,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
@@ -5559,7 +5562,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
@@ -5636,7 +5639,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
         <v>59</v>
       </c>
@@ -6024,7 +6027,7 @@
         <v>90</v>
       </c>
       <c r="V65" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W65" s="0" t="n">
         <v>20</v>
@@ -6104,7 +6107,7 @@
         <v>90</v>
       </c>
       <c r="V66" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W66" s="0" t="n">
         <v>20</v>
@@ -6436,7 +6439,7 @@
         <v>120</v>
       </c>
       <c r="V70" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W70" s="0" t="n">
         <v>20</v>
@@ -6688,7 +6691,7 @@
         <v>90</v>
       </c>
       <c r="V73" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W73" s="0" t="n">
         <v>20</v>
@@ -6768,7 +6771,7 @@
         <v>90</v>
       </c>
       <c r="V74" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W74" s="0" t="n">
         <v>20</v>
@@ -7005,7 +7008,7 @@
         <v>90</v>
       </c>
       <c r="V77" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W77" s="0" t="n">
         <v>20</v>
@@ -7085,7 +7088,7 @@
         <v>10</v>
       </c>
       <c r="V78" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="W78" s="0" t="n">
         <v>20</v>

</xml_diff>

<commit_message>
Update db + fix new sku type
</commit_message>
<xml_diff>
--- a/app/data/static/params/mozzarella.xlsx
+++ b/app/data/static/params/mozzarella.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="242">
   <si>
     <t xml:space="preserve">Название SKU</t>
   </si>
@@ -740,6 +740,12 @@
   </si>
   <si>
     <t xml:space="preserve">Н0000091462</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сулугуни в рассоле "Вкусвилл", 45%, 0,21/0,35 кг, ф/п</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00-00013255</t>
   </si>
 </sst>
 </file>
@@ -908,8 +914,8 @@
   </sheetPr>
   <dimension ref="A1:AD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B88" activeCellId="0" sqref="B88"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J74" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB89" activeCellId="0" sqref="AB89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8169,13 +8175,96 @@
       <c r="AA87" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="AB87" s="9" t="s">
+      <c r="AB87" s="6" t="s">
         <v>239</v>
       </c>
       <c r="AC87" s="0" t="n">
         <v>1300</v>
       </c>
       <c r="AD87" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E88" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F88" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G88" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H88" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="I88" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="J88" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K88" s="0" t="n">
+        <v>370</v>
+      </c>
+      <c r="L88" s="0" t="n">
+        <v>960</v>
+      </c>
+      <c r="M88" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="N88" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O88" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q88" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="R88" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="U88" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="V88" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="W88" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="X88" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y88" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z88" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA88" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB88" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="AC88" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="AD88" s="0" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>